<commit_message>
Update Rizka - 29 Mei 2020
</commit_message>
<xml_diff>
--- a/Data Binding Rizka.xlsx
+++ b/Data Binding Rizka.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\HunterCMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFCFB44-3CBB-4412-9834-EC17C304C281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30BE430-AE21-4743-BB58-FA1EAA22B98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="165" windowWidth="13410" windowHeight="11055" firstSheet="1" activeTab="2" xr2:uid="{32504A25-739A-48CD-B9AE-AF65002EA0BD}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13410" windowHeight="11055" firstSheet="2" activeTab="3" xr2:uid="{32504A25-739A-48CD-B9AE-AF65002EA0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Login - Logout" sheetId="1" r:id="rId1"/>
     <sheet name="FAQ Man - Delete FAQ" sheetId="2" r:id="rId2"/>
-    <sheet name="FAQ Man - New FAQ" sheetId="3" r:id="rId3"/>
+    <sheet name="FAQ Man - Add New FAQ" sheetId="3" r:id="rId3"/>
+    <sheet name="FAQ Man - Edit FAQ" sheetId="4" r:id="rId4"/>
+    <sheet name="FAQ Man - Search FAQ" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>username</t>
   </si>
@@ -68,13 +70,70 @@
   </si>
   <si>
     <t>FAQ2</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>Question New 1</t>
+  </si>
+  <si>
+    <t>Answer New 1</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>Question New 2</t>
+  </si>
+  <si>
+    <t>Answer New 3</t>
+  </si>
+  <si>
+    <t>Question New 4</t>
+  </si>
+  <si>
+    <t>Answer New 4</t>
+  </si>
+  <si>
+    <t>ABC LIMA DASAR</t>
+  </si>
+  <si>
+    <t>Apa itu PEOJF?</t>
+  </si>
+  <si>
+    <t>Question Edit 1</t>
+  </si>
+  <si>
+    <t>Question Edit 2</t>
+  </si>
+  <si>
+    <t>Answer Edit 1</t>
+  </si>
+  <si>
+    <t>Answer Edit 3</t>
+  </si>
+  <si>
+    <t>Question Edit 4</t>
+  </si>
+  <si>
+    <t>Answer Edit 4</t>
+  </si>
+  <si>
+    <t>questionBefore</t>
+  </si>
+  <si>
+    <t>questionAfter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +145,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -145,13 +219,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +556,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,60 +567,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -547,7 +634,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,26 +643,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -586,12 +673,218 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981E75B1-3FB0-49AC-AFF6-DDC68149952F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFBF645-8755-421E-8F9E-6D8EEF827F00}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF25EE9A-3B60-48CC-A9F0-015A5BA739B2}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>